<commit_message>
Launch Tests data added
</commit_message>
<xml_diff>
--- a/Lab5/Tests.xlsx
+++ b/Lab5/Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Academic Document\Class Materials\Fall 2019\ECSE-211-Design-Principles-and-Methods\Lab5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{54865DE0-A171-4DAD-A3F2-8BE577C27069}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E3A538D-B72B-4361-9E2C-6A5285EA343E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{BDAE5782-3F1A-4594-A0B3-CF635E36B1C5}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>MOTOR_SPEED</t>
   </si>
@@ -43,6 +43,15 @@
   </si>
   <si>
     <t>Turn 360 degrees</t>
+  </si>
+  <si>
+    <t>Launch_Angle</t>
+  </si>
+  <si>
+    <t>Acceleration</t>
+  </si>
+  <si>
+    <t>Range</t>
   </si>
 </sst>
 </file>
@@ -394,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABE12201-385F-4A38-A5B4-F6DD35547492}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -406,7 +415,7 @@
     <col min="2" max="2" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -419,8 +428,17 @@
       <c r="F1" t="s">
         <v>3</v>
       </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>100</v>
       </c>
@@ -433,8 +451,29 @@
       <c r="F2">
         <v>21</v>
       </c>
+      <c r="I2">
+        <v>45</v>
+      </c>
+      <c r="J2">
+        <v>3000</v>
+      </c>
+      <c r="K2">
+        <v>2.5</v>
+      </c>
+      <c r="L2">
+        <v>2.5</v>
+      </c>
+      <c r="M2">
+        <v>2.5</v>
+      </c>
+      <c r="N2">
+        <v>2.5</v>
+      </c>
+      <c r="O2">
+        <v>2.5</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>100</v>
       </c>
@@ -447,8 +486,29 @@
       <c r="F3">
         <v>18</v>
       </c>
+      <c r="I3">
+        <v>35</v>
+      </c>
+      <c r="J3">
+        <v>5000</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <v>2</v>
+      </c>
+      <c r="M3">
+        <v>2</v>
+      </c>
+      <c r="N3">
+        <v>2</v>
+      </c>
+      <c r="O3">
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>100</v>
       </c>
@@ -460,6 +520,96 @@
       </c>
       <c r="F4">
         <v>15</v>
+      </c>
+      <c r="I4">
+        <v>45</v>
+      </c>
+      <c r="J4">
+        <v>5000</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4">
+        <v>2</v>
+      </c>
+      <c r="M4">
+        <v>2</v>
+      </c>
+      <c r="N4">
+        <v>2</v>
+      </c>
+      <c r="O4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="I5">
+        <v>45</v>
+      </c>
+      <c r="J5">
+        <v>2750</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5">
+        <v>2</v>
+      </c>
+      <c r="M5">
+        <v>2</v>
+      </c>
+      <c r="N5">
+        <v>2</v>
+      </c>
+      <c r="O5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="I6">
+        <v>60</v>
+      </c>
+      <c r="J6">
+        <v>2750</v>
+      </c>
+      <c r="K6">
+        <v>1.5</v>
+      </c>
+      <c r="L6">
+        <v>1.5</v>
+      </c>
+      <c r="M6">
+        <v>1.5</v>
+      </c>
+      <c r="N6">
+        <v>1.5</v>
+      </c>
+      <c r="O6">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="I7">
+        <v>50</v>
+      </c>
+      <c r="J7">
+        <v>2750</v>
+      </c>
+      <c r="K7">
+        <v>2</v>
+      </c>
+      <c r="L7">
+        <v>2</v>
+      </c>
+      <c r="M7">
+        <v>2</v>
+      </c>
+      <c r="N7">
+        <v>2</v>
+      </c>
+      <c r="O7">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tuned catapult with solidified hardware design
</commit_message>
<xml_diff>
--- a/Lab5/Tests.xlsx
+++ b/Lab5/Tests.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Academic Document\Class Materials\Fall 2019\ECSE-211-Design-Principles-and-Methods\Lab5\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E3A538D-B72B-4361-9E2C-6A5285EA343E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{884FB891-EA80-47ED-854C-069D93ECE96D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{BDAE5782-3F1A-4594-A0B3-CF635E36B1C5}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="22716" windowHeight="13224" xr2:uid="{BDAE5782-3F1A-4594-A0B3-CF635E36B1C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -403,19 +399,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABE12201-385F-4A38-A5B4-F6DD35547492}">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K10" sqref="I1:O15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.19921875" customWidth="1"/>
+    <col min="1" max="1" width="17.21875" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -438,7 +434,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>100</v>
       </c>
@@ -473,7 +469,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>100</v>
       </c>
@@ -508,7 +504,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>100</v>
       </c>
@@ -543,7 +539,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="I5">
         <v>45</v>
       </c>
@@ -566,7 +562,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="I6">
         <v>60</v>
       </c>
@@ -589,7 +585,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="I7">
         <v>50</v>
       </c>
@@ -610,6 +606,190 @@
       </c>
       <c r="O7">
         <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="I8">
+        <v>75</v>
+      </c>
+      <c r="J8">
+        <v>2850</v>
+      </c>
+      <c r="K8">
+        <v>5.5</v>
+      </c>
+      <c r="L8">
+        <v>5.5</v>
+      </c>
+      <c r="M8">
+        <v>5.5</v>
+      </c>
+      <c r="N8">
+        <v>5.5</v>
+      </c>
+      <c r="O8">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="I9">
+        <v>65</v>
+      </c>
+      <c r="J9">
+        <v>2750</v>
+      </c>
+      <c r="K9">
+        <v>5.25</v>
+      </c>
+      <c r="L9">
+        <v>5.25</v>
+      </c>
+      <c r="M9">
+        <v>5.25</v>
+      </c>
+      <c r="N9">
+        <v>5.25</v>
+      </c>
+      <c r="O9">
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="I10">
+        <v>50</v>
+      </c>
+      <c r="J10">
+        <v>2750</v>
+      </c>
+      <c r="K10">
+        <v>5</v>
+      </c>
+      <c r="L10">
+        <v>5</v>
+      </c>
+      <c r="M10">
+        <v>5.25</v>
+      </c>
+      <c r="N10">
+        <v>5</v>
+      </c>
+      <c r="O10">
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="I11">
+        <v>50</v>
+      </c>
+      <c r="J11">
+        <v>2500</v>
+      </c>
+      <c r="K11">
+        <v>5</v>
+      </c>
+      <c r="L11">
+        <v>5</v>
+      </c>
+      <c r="M11">
+        <v>5</v>
+      </c>
+      <c r="N11">
+        <v>5</v>
+      </c>
+      <c r="O11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="I12">
+        <v>40</v>
+      </c>
+      <c r="J12">
+        <v>2500</v>
+      </c>
+      <c r="K12">
+        <v>5.25</v>
+      </c>
+      <c r="L12">
+        <v>5.25</v>
+      </c>
+      <c r="M12">
+        <v>5.25</v>
+      </c>
+      <c r="N12">
+        <v>5</v>
+      </c>
+      <c r="O12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="I13">
+        <v>40</v>
+      </c>
+      <c r="J13">
+        <v>2250</v>
+      </c>
+      <c r="K13">
+        <v>2.5</v>
+      </c>
+      <c r="L13">
+        <v>2.5</v>
+      </c>
+      <c r="M13">
+        <v>3</v>
+      </c>
+      <c r="N13">
+        <v>2</v>
+      </c>
+      <c r="O13">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="I14">
+        <v>40</v>
+      </c>
+      <c r="J14">
+        <v>2400</v>
+      </c>
+      <c r="K14">
+        <v>4.75</v>
+      </c>
+      <c r="L14">
+        <v>3</v>
+      </c>
+      <c r="M14">
+        <v>4.5</v>
+      </c>
+      <c r="N14">
+        <v>4.5</v>
+      </c>
+      <c r="O14">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="I15">
+        <v>40</v>
+      </c>
+      <c r="J15">
+        <v>2475</v>
+      </c>
+      <c r="K15">
+        <v>4.75</v>
+      </c>
+      <c r="L15">
+        <v>4.75</v>
+      </c>
+      <c r="M15">
+        <v>4.75</v>
+      </c>
+      <c r="N15">
+        <v>4.75</v>
+      </c>
+      <c r="O15">
+        <v>4.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>